<commit_message>
tabela-verdade-excel.xlsx: Grupos nos K-maps
</commit_message>
<xml_diff>
--- a/tabela-verdade-excel.xlsx
+++ b/tabela-verdade-excel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Leonardo\Documents\UFABC\22º QUAD - 2020.2 QS\Eletrônica Digital\Projeto Final\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E93CACB-A07B-40C6-BEDF-E3A96124D305}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CF8E087-D953-47AF-82F2-77BB3E7662A2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{F361B6BE-8EB6-4EE1-BE35-468091BD90C1}"/>
   </bookViews>
@@ -360,12 +360,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -396,14 +390,17 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="16">
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -457,6 +454,9 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -488,24 +488,2260 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo: Cantos Arredondados 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7CA33F91-6FBF-4037-86F5-7D687649F42C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12877800" y="561975"/>
+          <a:ext cx="1257300" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>600074</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Retângulo: Cantos Arredondados 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3570ACD8-7AC0-4C17-B16C-7BE4C0E5EFDA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11496674" y="971550"/>
+          <a:ext cx="2638425" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>619125</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Retângulo: Cantos Arredondados 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA38F1CA-D45B-43CE-BBBB-6F88E058E380}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12249150" y="781050"/>
+          <a:ext cx="1209675" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="60000"/>
+            <a:lumOff val="40000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>504826</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Retângulo: Cantos Arredondados 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B07D7B8F-05AA-4972-8C7B-BAF50A5D3FF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11534776" y="514350"/>
+          <a:ext cx="419100" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="7030A0">
+            <a:alpha val="32000"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>85726</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>504826</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Retângulo: Cantos Arredondados 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CE102697-822A-4FFF-8158-83C9B7A88965}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11534776" y="1133475"/>
+          <a:ext cx="419100" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="7030A0">
+            <a:alpha val="32000"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>9524</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="Retângulo: Cantos Arredondados 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AC334F2C-01F0-426D-ACBE-50F667292A5B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11553825" y="5000625"/>
+          <a:ext cx="2686049" cy="381000"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>685800</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="Retângulo: Cantos Arredondados 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1958A60-2FA2-4463-BCBE-64886BD5AB8F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12820650" y="4610100"/>
+          <a:ext cx="1400175" cy="238125"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="7030A0">
+            <a:alpha val="32000"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>47626</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>133351</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="Retângulo: Cantos Arredondados 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71B56D2E-402A-4280-94FC-993A59E623BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11496676" y="4581526"/>
+          <a:ext cx="657224" cy="257174"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="75000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>57151</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="Retângulo: Cantos Arredondados 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88A1F6C8-AC3B-40D6-9E20-889C765DC50F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11506201" y="5181600"/>
+          <a:ext cx="657224" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="75000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>676275</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="Retângulo: Cantos Arredondados 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B7B633A3-C5F2-4DF0-B309-D484047BA7E8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12220575" y="4829175"/>
+          <a:ext cx="600075" cy="419100"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="75000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>628650</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="Retângulo: Cantos Arredondados 12">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7361296E-D1F7-4984-96FB-EE8798CDC585}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13639800" y="4591050"/>
+          <a:ext cx="523875" cy="838200"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B0F0">
+            <a:alpha val="32000"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="14" name="Retângulo: Cantos Arredondados 13">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA424678-A5A5-45F2-B7F0-CF8C68CBE572}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11477625" y="1905000"/>
+          <a:ext cx="685800" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>676274</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="15" name="Retângulo: Cantos Arredondados 14">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6D411AF6-931A-470F-9DCB-37B718C28CFB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11496674" y="2295525"/>
+          <a:ext cx="2714625" cy="409575"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="7030A0">
+            <a:alpha val="32000"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="16" name="Retângulo: Cantos Arredondados 15">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{71AA45BB-F7FE-440F-A1D7-94DA056A07E0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12858750" y="1914525"/>
+          <a:ext cx="685800" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="75000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>666749</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="17" name="Retângulo: Cantos Arredondados 16">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BC216A0-CDD0-4D34-9218-FB9CA1CDA7DA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11487149" y="1914525"/>
+          <a:ext cx="2714625" cy="219075"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="18" name="Retângulo: Cantos Arredondados 17">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC8C8B7F-54D3-4BC3-A7EF-A6FDD67EC6CB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="12182475" y="3286125"/>
+          <a:ext cx="1419225" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="7030A0">
+            <a:alpha val="32000"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="19" name="Retângulo: Cantos Arredondados 18">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DDB5982-7DCC-4CF1-B52B-37BBF404DD05}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11506200" y="3267075"/>
+          <a:ext cx="638175" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>657224</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="20" name="Retângulo: Cantos Arredondados 19">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3BB1C193-7B0D-4B77-B53C-8A50C7991B70}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11477624" y="3457575"/>
+          <a:ext cx="2714625" cy="409575"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="75000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="21" name="Retângulo: Cantos Arredondados 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC3B2280-E87C-46CA-BBFA-E8B6F28F6DB4}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11639550" y="3676650"/>
+          <a:ext cx="2476500" cy="409575"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="00B0F0">
+            <a:alpha val="32000"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>19049</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>676274</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="Retângulo: Cantos Arredondados 21">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{78345484-0A13-4884-8CCA-EF3B1257E482}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18259424" y="571500"/>
+          <a:ext cx="657225" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>85724</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="Retângulo: Cantos Arredondados 22">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B9BA18F-1D8C-40CD-A269-E21E2ECC9817}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16240124" y="952500"/>
+          <a:ext cx="2657476" cy="228600"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>38099</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="Retângulo: Cantos Arredondados 23">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FCFCF44-EE81-4A29-8DD6-43A14D6EAFEA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16230599" y="542925"/>
+          <a:ext cx="657225" cy="257175"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="75000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>28574</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="Retângulo: Cantos Arredondados 24">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C624DA9-D310-416F-A6DE-BEFB621BDFB2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16221074" y="1133474"/>
+          <a:ext cx="657225" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="75000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="Retângulo: Cantos Arredondados 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3163758B-EC2E-4425-8BF3-D53B54AA7302}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17687925" y="1000125"/>
+          <a:ext cx="1209675" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="7030A0">
+            <a:alpha val="32000"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>666749</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="27" name="Retângulo: Cantos Arredondados 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CADF0C86-FD41-4340-BC42-F8F876426FEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16230599" y="2305050"/>
+          <a:ext cx="2676525" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>47624</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="28" name="Retângulo: Cantos Arredondados 27">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F3F3446-0045-4C93-AFB5-816FE86F4C13}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16316324" y="1943099"/>
+          <a:ext cx="400051" cy="809625"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:srgbClr val="7030A0">
+            <a:alpha val="32000"/>
+          </a:srgbClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>171449</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="29" name="Retângulo: Cantos Arredondados 28">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62C70CE7-C968-4C5A-9B9B-D94ACD88E3EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18411824" y="2114550"/>
+          <a:ext cx="600075" cy="409576"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>1209675</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>514351</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="30" name="Retângulo: Cantos Arredondados 29">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4A7D8A34-3112-4A09-98E5-114DE09DAB66}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16049625" y="2105025"/>
+          <a:ext cx="619126" cy="409576"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="31" name="Retângulo: Cantos Arredondados 30">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1207570B-2A80-480E-A74B-AEA34DD8E5CA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16402050" y="2133600"/>
+          <a:ext cx="1209675" cy="371475"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="75000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>47624</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>638174</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="32" name="Retângulo: Cantos Arredondados 31">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{422C5D3E-6F2C-4331-9AD3-E7671C8206EF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16202024" y="3676650"/>
+          <a:ext cx="2676525" cy="400050"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="Retângulo: Cantos Arredondados 32">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5BCFD2CF-E439-4F49-990A-BEB0A7FC20C7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="18335624" y="3267074"/>
+          <a:ext cx="485776" cy="828675"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent6">
+            <a:lumMod val="75000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>676274</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>19049</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="34" name="Retângulo: Cantos Arredondados 33">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7E573C36-54D3-4066-8D68-257F5857BF44}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17525999" y="3228975"/>
+          <a:ext cx="1476376" cy="266699"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="75000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>676274</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="35" name="Retângulo: Cantos Arredondados 34">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{114F2642-6D46-4AB2-B7F2-801CFFDD275C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="17525999" y="3829050"/>
+          <a:ext cx="1476376" cy="295275"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent2">
+            <a:lumMod val="75000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>590550</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>19051</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="36" name="Retângulo: Cantos Arredondados 35">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EFFC921-5416-410A-BCCE-6E35E7AC85D5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16297274" y="3467100"/>
+          <a:ext cx="1143001" cy="409576"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent4">
+            <a:lumMod val="75000"/>
+            <a:alpha val="32000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="pt-BR" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6156926B-C7CC-4E37-8D94-56C92610D964}" name="Tabela1" displayName="Tabela1" ref="B2:O13" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
   <autoFilter ref="B2:O13" xr:uid="{D80E1C1D-81A5-4C2C-8B80-CE49B71DD167}"/>
   <tableColumns count="14">
-    <tableColumn id="14" xr3:uid="{CE384D31-85BA-4DD1-93B9-EC31873B87AC}" name="NUM" dataDxfId="0"/>
-    <tableColumn id="1" xr3:uid="{EBD275CE-22DE-4DBE-AA3C-991F0247F9CD}" name="BCD_IN[3]" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{A3471ECF-46BC-4198-9C1A-B7817C996064}" name="BCD_IN[2]" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{EDDE83D1-691C-480B-9FD5-90ABC760B2E9}" name="BCD_IN[1]" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{B9A7C817-B561-4205-9FF2-4F5112D52D12}" name="BCD_IN[0]" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{7D5948E6-BD82-4274-8041-FA1A7B122E10}" name="RST" dataDxfId="9"/>
-    <tableColumn id="6" xr3:uid="{2EAAC2EE-C899-4A74-A057-2C7306B5B743}" name="A" dataDxfId="8"/>
-    <tableColumn id="7" xr3:uid="{8CC9A0BA-0EAA-4659-BB4F-3A7098541925}" name="B" dataDxfId="7"/>
-    <tableColumn id="8" xr3:uid="{3431AC04-3006-4B7D-BEE1-95B5264CE454}" name="C" dataDxfId="6"/>
-    <tableColumn id="9" xr3:uid="{50953F91-2BA0-4B61-BDAB-1EDBBC8E33DF}" name="D" dataDxfId="5"/>
-    <tableColumn id="10" xr3:uid="{A0CC7459-8A81-4B09-A1C1-12C054249B01}" name="E" dataDxfId="4"/>
-    <tableColumn id="11" xr3:uid="{F361C4EB-1F17-4EC3-8088-A17366EABE29}" name="F" dataDxfId="3"/>
-    <tableColumn id="12" xr3:uid="{666BE741-6D80-4216-B3B0-13FEEA4C515E}" name="G" dataDxfId="2"/>
-    <tableColumn id="13" xr3:uid="{529A0E3B-06A4-4971-AB14-E810A5DE4142}" name="DP" dataDxfId="1"/>
+    <tableColumn id="14" xr3:uid="{CE384D31-85BA-4DD1-93B9-EC31873B87AC}" name="NUM" dataDxfId="13"/>
+    <tableColumn id="1" xr3:uid="{EBD275CE-22DE-4DBE-AA3C-991F0247F9CD}" name="BCD_IN[3]" dataDxfId="12"/>
+    <tableColumn id="2" xr3:uid="{A3471ECF-46BC-4198-9C1A-B7817C996064}" name="BCD_IN[2]" dataDxfId="11"/>
+    <tableColumn id="3" xr3:uid="{EDDE83D1-691C-480B-9FD5-90ABC760B2E9}" name="BCD_IN[1]" dataDxfId="10"/>
+    <tableColumn id="4" xr3:uid="{B9A7C817-B561-4205-9FF2-4F5112D52D12}" name="BCD_IN[0]" dataDxfId="9"/>
+    <tableColumn id="5" xr3:uid="{7D5948E6-BD82-4274-8041-FA1A7B122E10}" name="RST" dataDxfId="8"/>
+    <tableColumn id="6" xr3:uid="{2EAAC2EE-C899-4A74-A057-2C7306B5B743}" name="A" dataDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{8CC9A0BA-0EAA-4659-BB4F-3A7098541925}" name="B" dataDxfId="6"/>
+    <tableColumn id="8" xr3:uid="{3431AC04-3006-4B7D-BEE1-95B5264CE454}" name="C" dataDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{50953F91-2BA0-4B61-BDAB-1EDBBC8E33DF}" name="D" dataDxfId="4"/>
+    <tableColumn id="10" xr3:uid="{A0CC7459-8A81-4B09-A1C1-12C054249B01}" name="E" dataDxfId="3"/>
+    <tableColumn id="11" xr3:uid="{F361C4EB-1F17-4EC3-8088-A17366EABE29}" name="F" dataDxfId="2"/>
+    <tableColumn id="12" xr3:uid="{666BE741-6D80-4216-B3B0-13FEEA4C515E}" name="G" dataDxfId="1"/>
+    <tableColumn id="13" xr3:uid="{529A0E3B-06A4-4971-AB14-E810A5DE4142}" name="DP" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -830,8 +3066,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7F9A624-3E48-4BE7-89A1-AAA6F4C86DA1}">
   <dimension ref="B1:AA28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I17" sqref="I17"/>
+    <sheetView tabSelected="1" topLeftCell="J4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Y24" sqref="Y24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -901,21 +3137,21 @@
       <c r="Q2" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="R2" s="11" t="s">
+      <c r="R2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="S2" s="11"/>
-      <c r="T2" s="11"/>
-      <c r="U2" s="12"/>
+      <c r="S2" s="21"/>
+      <c r="T2" s="21"/>
+      <c r="U2" s="22"/>
       <c r="W2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="X2" s="11" t="s">
+      <c r="X2" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="Y2" s="11"/>
-      <c r="Z2" s="11"/>
-      <c r="AA2" s="12"/>
+      <c r="Y2" s="21"/>
+      <c r="Z2" s="21"/>
+      <c r="AA2" s="22"/>
     </row>
     <row r="3" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B3" s="2">
@@ -960,34 +3196,34 @@
       <c r="O3" s="2">
         <v>1</v>
       </c>
-      <c r="Q3" s="13" t="s">
+      <c r="Q3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="R3" s="14" t="s">
+      <c r="R3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="S3" s="14" t="s">
+      <c r="S3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="T3" s="14" t="s">
+      <c r="T3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="U3" s="15" t="s">
+      <c r="U3" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="W3" s="13" t="s">
+      <c r="W3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="X3" s="14" t="s">
+      <c r="X3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="Y3" s="14" t="s">
+      <c r="Y3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="Z3" s="14" t="s">
+      <c r="Z3" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AA3" s="15" t="s">
+      <c r="AA3" s="13" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1034,7 +3270,7 @@
       <c r="O4" s="2">
         <v>1</v>
       </c>
-      <c r="Q4" s="16" t="s">
+      <c r="Q4" s="14" t="s">
         <v>17</v>
       </c>
       <c r="R4" s="8">
@@ -1046,10 +3282,10 @@
       <c r="T4" s="8">
         <v>1</v>
       </c>
-      <c r="U4" s="17">
-        <v>1</v>
-      </c>
-      <c r="W4" s="16" t="s">
+      <c r="U4" s="15">
+        <v>1</v>
+      </c>
+      <c r="W4" s="14" t="s">
         <v>17</v>
       </c>
       <c r="X4" s="8">
@@ -1061,7 +3297,7 @@
       <c r="Z4" s="8">
         <v>0</v>
       </c>
-      <c r="AA4" s="17">
+      <c r="AA4" s="15">
         <v>1</v>
       </c>
     </row>
@@ -1108,7 +3344,7 @@
       <c r="O5" s="2">
         <v>1</v>
       </c>
-      <c r="Q5" s="18" t="s">
+      <c r="Q5" s="16" t="s">
         <v>18</v>
       </c>
       <c r="R5" s="9">
@@ -1120,10 +3356,10 @@
       <c r="T5" s="9">
         <v>1</v>
       </c>
-      <c r="U5" s="19">
-        <v>1</v>
-      </c>
-      <c r="W5" s="18" t="s">
+      <c r="U5" s="17">
+        <v>1</v>
+      </c>
+      <c r="W5" s="16" t="s">
         <v>18</v>
       </c>
       <c r="X5" s="9">
@@ -1135,7 +3371,7 @@
       <c r="Z5" s="9">
         <v>0</v>
       </c>
-      <c r="AA5" s="19">
+      <c r="AA5" s="17">
         <v>1</v>
       </c>
     </row>
@@ -1182,7 +3418,7 @@
       <c r="O6" s="2">
         <v>1</v>
       </c>
-      <c r="Q6" s="18" t="s">
+      <c r="Q6" s="16" t="s">
         <v>19</v>
       </c>
       <c r="R6" s="9">
@@ -1194,10 +3430,10 @@
       <c r="T6" s="9">
         <v>1</v>
       </c>
-      <c r="U6" s="19">
-        <v>1</v>
-      </c>
-      <c r="W6" s="18" t="s">
+      <c r="U6" s="17">
+        <v>1</v>
+      </c>
+      <c r="W6" s="16" t="s">
         <v>19</v>
       </c>
       <c r="X6" s="9">
@@ -1209,7 +3445,7 @@
       <c r="Z6" s="9">
         <v>1</v>
       </c>
-      <c r="AA6" s="19">
+      <c r="AA6" s="17">
         <v>1</v>
       </c>
     </row>
@@ -1256,34 +3492,34 @@
       <c r="O7" s="2">
         <v>1</v>
       </c>
-      <c r="Q7" s="20" t="s">
+      <c r="Q7" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="R7" s="21">
-        <v>1</v>
-      </c>
-      <c r="S7" s="21">
-        <v>1</v>
-      </c>
-      <c r="T7" s="21">
-        <v>1</v>
-      </c>
-      <c r="U7" s="22">
-        <v>1</v>
-      </c>
-      <c r="W7" s="20" t="s">
+      <c r="R7" s="19">
+        <v>1</v>
+      </c>
+      <c r="S7" s="19">
+        <v>1</v>
+      </c>
+      <c r="T7" s="19">
+        <v>1</v>
+      </c>
+      <c r="U7" s="20">
+        <v>1</v>
+      </c>
+      <c r="W7" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="X7" s="21">
-        <v>1</v>
-      </c>
-      <c r="Y7" s="21">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="21">
-        <v>1</v>
-      </c>
-      <c r="AA7" s="22">
+      <c r="X7" s="19">
+        <v>1</v>
+      </c>
+      <c r="Y7" s="19">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="19">
+        <v>1</v>
+      </c>
+      <c r="AA7" s="20">
         <v>1</v>
       </c>
     </row>
@@ -1377,21 +3613,21 @@
       <c r="Q9" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="R9" s="11" t="s">
+      <c r="R9" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="12"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="21"/>
+      <c r="U9" s="22"/>
       <c r="W9" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="X9" s="11" t="s">
+      <c r="X9" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="Y9" s="11"/>
-      <c r="Z9" s="11"/>
-      <c r="AA9" s="12"/>
+      <c r="Y9" s="21"/>
+      <c r="Z9" s="21"/>
+      <c r="AA9" s="22"/>
     </row>
     <row r="10" spans="2:27" x14ac:dyDescent="0.25">
       <c r="B10" s="2">
@@ -1436,34 +3672,34 @@
       <c r="O10" s="2">
         <v>1</v>
       </c>
-      <c r="Q10" s="13" t="s">
+      <c r="Q10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="R10" s="14" t="s">
+      <c r="R10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="S10" s="14" t="s">
+      <c r="S10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="T10" s="14" t="s">
+      <c r="T10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="U10" s="15" t="s">
+      <c r="U10" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="W10" s="13" t="s">
+      <c r="W10" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="X10" s="14" t="s">
+      <c r="X10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="Y10" s="14" t="s">
+      <c r="Y10" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="Z10" s="14" t="s">
+      <c r="Z10" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AA10" s="15" t="s">
+      <c r="AA10" s="13" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1510,7 +3746,7 @@
       <c r="O11" s="2">
         <v>1</v>
       </c>
-      <c r="Q11" s="16" t="s">
+      <c r="Q11" s="14" t="s">
         <v>17</v>
       </c>
       <c r="R11" s="8">
@@ -1522,10 +3758,10 @@
       <c r="T11" s="8">
         <v>1</v>
       </c>
-      <c r="U11" s="17">
-        <v>1</v>
-      </c>
-      <c r="W11" s="16" t="s">
+      <c r="U11" s="15">
+        <v>1</v>
+      </c>
+      <c r="W11" s="14" t="s">
         <v>17</v>
       </c>
       <c r="X11" s="8">
@@ -1537,7 +3773,7 @@
       <c r="Z11" s="8">
         <v>0</v>
       </c>
-      <c r="AA11" s="17">
+      <c r="AA11" s="15">
         <v>0</v>
       </c>
     </row>
@@ -1584,7 +3820,7 @@
       <c r="O12" s="2">
         <v>1</v>
       </c>
-      <c r="Q12" s="18" t="s">
+      <c r="Q12" s="16" t="s">
         <v>18</v>
       </c>
       <c r="R12" s="9">
@@ -1596,10 +3832,10 @@
       <c r="T12" s="9">
         <v>1</v>
       </c>
-      <c r="U12" s="19">
-        <v>0</v>
-      </c>
-      <c r="W12" s="18" t="s">
+      <c r="U12" s="17">
+        <v>0</v>
+      </c>
+      <c r="W12" s="16" t="s">
         <v>18</v>
       </c>
       <c r="X12" s="9">
@@ -1611,7 +3847,7 @@
       <c r="Z12" s="9">
         <v>0</v>
       </c>
-      <c r="AA12" s="19">
+      <c r="AA12" s="17">
         <v>1</v>
       </c>
     </row>
@@ -1658,7 +3894,7 @@
       <c r="O13" s="5">
         <v>1</v>
       </c>
-      <c r="Q13" s="18" t="s">
+      <c r="Q13" s="16" t="s">
         <v>19</v>
       </c>
       <c r="R13" s="9">
@@ -1670,10 +3906,10 @@
       <c r="T13" s="9">
         <v>1</v>
       </c>
-      <c r="U13" s="19">
-        <v>1</v>
-      </c>
-      <c r="W13" s="18" t="s">
+      <c r="U13" s="17">
+        <v>1</v>
+      </c>
+      <c r="W13" s="16" t="s">
         <v>19</v>
       </c>
       <c r="X13" s="9">
@@ -1685,39 +3921,39 @@
       <c r="Z13" s="9">
         <v>1</v>
       </c>
-      <c r="AA13" s="19">
+      <c r="AA13" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="14" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q14" s="20" t="s">
+      <c r="Q14" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="R14" s="21">
-        <v>1</v>
-      </c>
-      <c r="S14" s="21">
-        <v>1</v>
-      </c>
-      <c r="T14" s="21">
-        <v>1</v>
-      </c>
-      <c r="U14" s="22">
-        <v>1</v>
-      </c>
-      <c r="W14" s="20" t="s">
+      <c r="R14" s="19">
+        <v>1</v>
+      </c>
+      <c r="S14" s="19">
+        <v>1</v>
+      </c>
+      <c r="T14" s="19">
+        <v>1</v>
+      </c>
+      <c r="U14" s="20">
+        <v>1</v>
+      </c>
+      <c r="W14" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="X14" s="21">
-        <v>1</v>
-      </c>
-      <c r="Y14" s="21">
-        <v>1</v>
-      </c>
-      <c r="Z14" s="21">
-        <v>1</v>
-      </c>
-      <c r="AA14" s="22">
+      <c r="X14" s="19">
+        <v>1</v>
+      </c>
+      <c r="Y14" s="19">
+        <v>1</v>
+      </c>
+      <c r="Z14" s="19">
+        <v>1</v>
+      </c>
+      <c r="AA14" s="20">
         <v>1</v>
       </c>
     </row>
@@ -1726,56 +3962,56 @@
       <c r="Q16" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="R16" s="11" t="s">
+      <c r="R16" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="S16" s="11"/>
-      <c r="T16" s="11"/>
-      <c r="U16" s="12"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="21"/>
+      <c r="U16" s="22"/>
       <c r="W16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="X16" s="11" t="s">
+      <c r="X16" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="Y16" s="11"/>
-      <c r="Z16" s="11"/>
-      <c r="AA16" s="12"/>
+      <c r="Y16" s="21"/>
+      <c r="Z16" s="21"/>
+      <c r="AA16" s="22"/>
     </row>
     <row r="17" spans="17:27" x14ac:dyDescent="0.25">
-      <c r="Q17" s="13" t="s">
+      <c r="Q17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="R17" s="14" t="s">
+      <c r="R17" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="S17" s="14" t="s">
+      <c r="S17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="T17" s="14" t="s">
+      <c r="T17" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="U17" s="15" t="s">
+      <c r="U17" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="W17" s="13" t="s">
+      <c r="W17" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="X17" s="14" t="s">
+      <c r="X17" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="Y17" s="14" t="s">
+      <c r="Y17" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="Z17" s="14" t="s">
+      <c r="Z17" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AA17" s="15" t="s">
+      <c r="AA17" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="18" spans="17:27" x14ac:dyDescent="0.25">
-      <c r="Q18" s="16" t="s">
+      <c r="Q18" s="14" t="s">
         <v>17</v>
       </c>
       <c r="R18" s="8">
@@ -1787,10 +4023,10 @@
       <c r="T18" s="8">
         <v>1</v>
       </c>
-      <c r="U18" s="17">
-        <v>0</v>
-      </c>
-      <c r="W18" s="16" t="s">
+      <c r="U18" s="15">
+        <v>0</v>
+      </c>
+      <c r="W18" s="14" t="s">
         <v>17</v>
       </c>
       <c r="X18" s="8">
@@ -1802,12 +4038,12 @@
       <c r="Z18" s="8">
         <v>1</v>
       </c>
-      <c r="AA18" s="17">
+      <c r="AA18" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="19" spans="17:27" x14ac:dyDescent="0.25">
-      <c r="Q19" s="18" t="s">
+      <c r="Q19" s="16" t="s">
         <v>18</v>
       </c>
       <c r="R19" s="9">
@@ -1819,10 +4055,10 @@
       <c r="T19" s="9">
         <v>1</v>
       </c>
-      <c r="U19" s="19">
-        <v>1</v>
-      </c>
-      <c r="W19" s="18" t="s">
+      <c r="U19" s="17">
+        <v>1</v>
+      </c>
+      <c r="W19" s="16" t="s">
         <v>18</v>
       </c>
       <c r="X19" s="9">
@@ -1834,12 +4070,12 @@
       <c r="Z19" s="9">
         <v>0</v>
       </c>
-      <c r="AA19" s="19">
+      <c r="AA19" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="20" spans="17:27" x14ac:dyDescent="0.25">
-      <c r="Q20" s="18" t="s">
+      <c r="Q20" s="16" t="s">
         <v>19</v>
       </c>
       <c r="R20" s="9">
@@ -1851,10 +4087,10 @@
       <c r="T20" s="9">
         <v>1</v>
       </c>
-      <c r="U20" s="19">
-        <v>1</v>
-      </c>
-      <c r="W20" s="18" t="s">
+      <c r="U20" s="17">
+        <v>1</v>
+      </c>
+      <c r="W20" s="16" t="s">
         <v>19</v>
       </c>
       <c r="X20" s="9">
@@ -1866,39 +4102,39 @@
       <c r="Z20" s="9">
         <v>1</v>
       </c>
-      <c r="AA20" s="19">
+      <c r="AA20" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="21" spans="17:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q21" s="20" t="s">
+      <c r="Q21" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="R21" s="21">
-        <v>1</v>
-      </c>
-      <c r="S21" s="21">
-        <v>1</v>
-      </c>
-      <c r="T21" s="21">
-        <v>1</v>
-      </c>
-      <c r="U21" s="22">
-        <v>1</v>
-      </c>
-      <c r="W21" s="20" t="s">
+      <c r="R21" s="19">
+        <v>1</v>
+      </c>
+      <c r="S21" s="19">
+        <v>1</v>
+      </c>
+      <c r="T21" s="19">
+        <v>1</v>
+      </c>
+      <c r="U21" s="20">
+        <v>1</v>
+      </c>
+      <c r="W21" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="X21" s="21">
-        <v>1</v>
-      </c>
-      <c r="Y21" s="21">
-        <v>1</v>
-      </c>
-      <c r="Z21" s="21">
-        <v>1</v>
-      </c>
-      <c r="AA21" s="22">
+      <c r="X21" s="19">
+        <v>1</v>
+      </c>
+      <c r="Y21" s="19">
+        <v>1</v>
+      </c>
+      <c r="Z21" s="19">
+        <v>1</v>
+      </c>
+      <c r="AA21" s="20">
         <v>1</v>
       </c>
     </row>
@@ -1907,12 +4143,12 @@
       <c r="Q23" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="R23" s="11" t="s">
+      <c r="R23" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="S23" s="11"/>
-      <c r="T23" s="11"/>
-      <c r="U23" s="12"/>
+      <c r="S23" s="21"/>
+      <c r="T23" s="21"/>
+      <c r="U23" s="22"/>
       <c r="W23"/>
       <c r="X23"/>
       <c r="Y23"/>
@@ -1920,19 +4156,19 @@
       <c r="AA23"/>
     </row>
     <row r="24" spans="17:27" x14ac:dyDescent="0.25">
-      <c r="Q24" s="13" t="s">
+      <c r="Q24" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="R24" s="14" t="s">
+      <c r="R24" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="S24" s="14" t="s">
+      <c r="S24" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="T24" s="14" t="s">
+      <c r="T24" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="U24" s="15" t="s">
+      <c r="U24" s="13" t="s">
         <v>20</v>
       </c>
       <c r="W24"/>
@@ -1942,7 +4178,7 @@
       <c r="AA24"/>
     </row>
     <row r="25" spans="17:27" x14ac:dyDescent="0.25">
-      <c r="Q25" s="16" t="s">
+      <c r="Q25" s="14" t="s">
         <v>17</v>
       </c>
       <c r="R25" s="8">
@@ -1954,7 +4190,7 @@
       <c r="T25" s="8">
         <v>1</v>
       </c>
-      <c r="U25" s="17">
+      <c r="U25" s="15">
         <v>1</v>
       </c>
       <c r="W25"/>
@@ -1964,7 +4200,7 @@
       <c r="AA25"/>
     </row>
     <row r="26" spans="17:27" x14ac:dyDescent="0.25">
-      <c r="Q26" s="18" t="s">
+      <c r="Q26" s="16" t="s">
         <v>18</v>
       </c>
       <c r="R26" s="9">
@@ -1974,9 +4210,9 @@
         <v>1</v>
       </c>
       <c r="T26" s="9">
-        <v>1</v>
-      </c>
-      <c r="U26" s="19">
+        <v>0</v>
+      </c>
+      <c r="U26" s="17">
         <v>1</v>
       </c>
       <c r="W26"/>
@@ -1986,7 +4222,7 @@
       <c r="AA26"/>
     </row>
     <row r="27" spans="17:27" x14ac:dyDescent="0.25">
-      <c r="Q27" s="18" t="s">
+      <c r="Q27" s="16" t="s">
         <v>19</v>
       </c>
       <c r="R27" s="9">
@@ -1998,7 +4234,7 @@
       <c r="T27" s="9">
         <v>1</v>
       </c>
-      <c r="U27" s="19">
+      <c r="U27" s="17">
         <v>1</v>
       </c>
       <c r="W27"/>
@@ -2008,19 +4244,19 @@
       <c r="AA27"/>
     </row>
     <row r="28" spans="17:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="Q28" s="20" t="s">
+      <c r="Q28" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="R28" s="21">
-        <v>1</v>
-      </c>
-      <c r="S28" s="21">
-        <v>1</v>
-      </c>
-      <c r="T28" s="21">
-        <v>1</v>
-      </c>
-      <c r="U28" s="22">
+      <c r="R28" s="19">
+        <v>1</v>
+      </c>
+      <c r="S28" s="19">
+        <v>1</v>
+      </c>
+      <c r="T28" s="19">
+        <v>1</v>
+      </c>
+      <c r="U28" s="20">
         <v>1</v>
       </c>
       <c r="W28"/>
@@ -2031,21 +4267,22 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="X2:AA2"/>
     <mergeCell ref="R9:U9"/>
     <mergeCell ref="X9:AA9"/>
     <mergeCell ref="R16:U16"/>
     <mergeCell ref="R23:U23"/>
     <mergeCell ref="X16:AA16"/>
-    <mergeCell ref="R2:U2"/>
-    <mergeCell ref="X2:AA2"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="Q4:Q21 R4:U21 R3:AA3 V4:AA21 Q23:U28" numberStoredAsText="1"/>
+    <ignoredError sqref="Q4:Q21 R4:U21 R3:AA3 V4:AA21 Q23:U25 Q27:U28 Q26:S26 U26" numberStoredAsText="1"/>
   </ignoredErrors>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>

</xml_diff>